<commit_message>
theoretical lipid MS1 searching in raw lipidex results
</commit_message>
<xml_diff>
--- a/data/metadata/animal_phenotypes.xlsx
+++ b/data/metadata/animal_phenotypes.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nile_rat_multiomics\data\metadata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62285CEC-1E67-4D0F-95FB-CF6E5F82DBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>Date of birth</t>
   </si>
@@ -208,9 +214,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>ogtt_rank</t>
-  </si>
-  <si>
     <t>animal</t>
   </si>
   <si>
@@ -254,46 +257,16 @@
   </si>
   <si>
     <t>euthanized</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +330,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -403,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,9 +416,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,6 +468,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -644,16 +661,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BN20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AV29" sqref="AV29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:66">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -847,11 +869,8 @@
       <c r="BM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="1" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="2" spans="1:66">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1060</v>
       </c>
@@ -865,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>58.5</v>
@@ -889,28 +908,28 @@
         <v>48742.5</v>
       </c>
       <c r="M2">
-        <v>2.358</v>
+        <v>2.3580000000000001</v>
       </c>
       <c r="N2">
-        <v>2.154</v>
+        <v>2.1539999999999999</v>
       </c>
       <c r="O2">
-        <v>2.537</v>
+        <v>2.5369999999999999</v>
       </c>
       <c r="P2">
-        <v>2.207</v>
+        <v>2.2069999999999999</v>
       </c>
       <c r="Q2">
-        <v>3.396</v>
+        <v>3.3959999999999999</v>
       </c>
       <c r="R2">
-        <v>5.576</v>
+        <v>5.5759999999999996</v>
       </c>
       <c r="S2">
-        <v>422.939999999999</v>
+        <v>422.93999999999897</v>
       </c>
       <c r="T2">
-        <v>71.00000009999999</v>
+        <v>71.000000099999994</v>
       </c>
       <c r="U2">
         <v>225</v>
@@ -943,19 +962,19 @@
         <v>58.5</v>
       </c>
       <c r="AE2">
-        <v>2.874</v>
+        <v>2.8740000000000001</v>
       </c>
       <c r="AF2">
-        <v>1.668</v>
+        <v>1.6679999999999999</v>
       </c>
       <c r="AG2">
-        <v>0.9635</v>
+        <v>0.96350000000000002</v>
       </c>
       <c r="AH2">
-        <v>1.414</v>
+        <v>1.4139999999999999</v>
       </c>
       <c r="AI2">
-        <v>2.358</v>
+        <v>2.3580000000000001</v>
       </c>
       <c r="AJ2">
         <v>11.42</v>
@@ -976,10 +995,10 @@
         <v>53.7</v>
       </c>
       <c r="AP2">
-        <v>92.59999999999999</v>
+        <v>92.6</v>
       </c>
       <c r="AQ2">
-        <v>98.09999999999999</v>
+        <v>98.1</v>
       </c>
       <c r="AR2">
         <v>100.9</v>
@@ -991,13 +1010,13 @@
         <v>104.6</v>
       </c>
       <c r="AU2">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="AV2">
-        <v>90.90000000000001</v>
+        <v>90.9</v>
       </c>
       <c r="AW2">
-        <v>94.90000000000001</v>
+        <v>94.9</v>
       </c>
       <c r="AX2">
         <v>99.5</v>
@@ -1027,25 +1046,22 @@
         <v>1.94557564224548</v>
       </c>
       <c r="BH2">
-        <v>0.7185</v>
+        <v>0.71850000000000003</v>
       </c>
       <c r="BI2">
-        <v>0.6836346336822074</v>
+        <v>0.68363463368220745</v>
       </c>
       <c r="BJ2">
-        <v>2.845929018789144</v>
+        <v>2.8459290187891439</v>
       </c>
       <c r="BK2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL2" t="s">
-        <v>72</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:66">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1061</v>
       </c>
@@ -1080,22 +1096,22 @@
         <v>46485</v>
       </c>
       <c r="M3">
-        <v>3.087</v>
+        <v>3.0870000000000002</v>
       </c>
       <c r="N3">
         <v>2.407</v>
       </c>
       <c r="O3">
-        <v>1.783</v>
+        <v>1.7829999999999999</v>
       </c>
       <c r="P3">
         <v>1.425</v>
       </c>
       <c r="Q3">
-        <v>2.155</v>
+        <v>2.1549999999999998</v>
       </c>
       <c r="R3">
-        <v>2.648</v>
+        <v>2.6480000000000001</v>
       </c>
       <c r="S3">
         <v>262.25</v>
@@ -1146,19 +1162,19 @@
         <v>1.681</v>
       </c>
       <c r="AI3">
-        <v>3.087</v>
+        <v>3.0870000000000002</v>
       </c>
       <c r="AJ3">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="AK3">
         <v>13.42</v>
       </c>
       <c r="AL3">
-        <v>9.667</v>
+        <v>9.6669999999999998</v>
       </c>
       <c r="AM3">
-        <v>6.699</v>
+        <v>6.6989999999999998</v>
       </c>
       <c r="AN3">
         <v>48.37</v>
@@ -1167,10 +1183,10 @@
         <v>52.1</v>
       </c>
       <c r="AP3">
-        <v>88.90000000000001</v>
+        <v>88.9</v>
       </c>
       <c r="AQ3">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="AR3">
         <v>98.2</v>
@@ -1197,7 +1213,7 @@
         <v>101.7</v>
       </c>
       <c r="AZ3">
-        <v>85.90000000000001</v>
+        <v>85.9</v>
       </c>
       <c r="BA3">
         <v>90.7</v>
@@ -1206,34 +1222,34 @@
         <v>97</v>
       </c>
       <c r="BC3">
-        <v>98.09999999999999</v>
+        <v>98.1</v>
       </c>
       <c r="BD3">
         <v>101.7</v>
       </c>
       <c r="BF3">
-        <v>1.7808</v>
+        <v>1.7807999999999999</v>
       </c>
       <c r="BG3">
         <v>1.751032448377581</v>
       </c>
       <c r="BH3">
-        <v>0.6059</v>
+        <v>0.60589999999999999</v>
       </c>
       <c r="BI3">
-        <v>0.595771878072763</v>
+        <v>0.59577187807276299</v>
       </c>
       <c r="BJ3">
-        <v>2.939098861198218</v>
+        <v>2.9390988611982181</v>
       </c>
       <c r="BK3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:66">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1062</v>
       </c>
@@ -1247,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <v>56.5</v>
@@ -1271,22 +1287,22 @@
         <v>43717.5</v>
       </c>
       <c r="M4">
-        <v>3.344</v>
+        <v>3.3439999999999999</v>
       </c>
       <c r="N4">
-        <v>2.591</v>
+        <v>2.5910000000000002</v>
       </c>
       <c r="O4">
-        <v>3.498</v>
+        <v>3.4980000000000002</v>
       </c>
       <c r="P4">
-        <v>2.878</v>
+        <v>2.8780000000000001</v>
       </c>
       <c r="Q4">
-        <v>3.076</v>
+        <v>3.0760000000000001</v>
       </c>
       <c r="R4">
-        <v>5.281</v>
+        <v>5.2809999999999997</v>
       </c>
       <c r="S4">
         <v>432.02</v>
@@ -1307,10 +1323,10 @@
         <v>248.5</v>
       </c>
       <c r="Y4">
-        <v>90.33333333333333</v>
+        <v>90.333333333333329</v>
       </c>
       <c r="Z4">
-        <v>52.33333333333334</v>
+        <v>52.333333333333343</v>
       </c>
       <c r="AA4">
         <v>48</v>
@@ -1325,19 +1341,19 @@
         <v>56.5</v>
       </c>
       <c r="AE4">
-        <v>4.154</v>
+        <v>4.1539999999999999</v>
       </c>
       <c r="AF4">
         <v>2.879</v>
       </c>
       <c r="AG4">
-        <v>1.977</v>
+        <v>1.9770000000000001</v>
       </c>
       <c r="AH4">
         <v>2.734</v>
       </c>
       <c r="AI4">
-        <v>3.344</v>
+        <v>3.3439999999999999</v>
       </c>
       <c r="AJ4">
         <v>10.37</v>
@@ -1349,7 +1365,7 @@
         <v>11.56</v>
       </c>
       <c r="AM4">
-        <v>9.449999999999999</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="AN4">
         <v>38.47</v>
@@ -1376,7 +1392,7 @@
         <v>86.7</v>
       </c>
       <c r="AV4">
-        <v>91.90000000000001</v>
+        <v>91.9</v>
       </c>
       <c r="AW4">
         <v>96.8</v>
@@ -1391,7 +1407,7 @@
         <v>91.2</v>
       </c>
       <c r="BA4">
-        <v>96.09999999999999</v>
+        <v>96.1</v>
       </c>
       <c r="BB4">
         <v>101.3</v>
@@ -1409,25 +1425,22 @@
         <v>2.308432630614115</v>
       </c>
       <c r="BH4">
-        <v>0.7439</v>
+        <v>0.74390000000000001</v>
       </c>
       <c r="BI4">
-        <v>0.6818515123739688</v>
+        <v>0.68185151237396879</v>
       </c>
       <c r="BJ4">
-        <v>3.385535690280952</v>
+        <v>3.3855356902809519</v>
       </c>
       <c r="BK4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:66">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1063</v>
       </c>
@@ -1441,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>4.366</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="T5">
         <v>73</v>
@@ -1474,19 +1487,19 @@
         <v>42</v>
       </c>
       <c r="AE5">
-        <v>2.304</v>
+        <v>2.3039999999999998</v>
       </c>
       <c r="AF5">
-        <v>0.9952</v>
+        <v>0.99519999999999997</v>
       </c>
       <c r="AG5">
         <v>1.381</v>
       </c>
       <c r="AH5">
-        <v>2.53</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="AI5">
-        <v>4.366</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="AJ5">
         <v>43.94</v>
@@ -1504,7 +1517,7 @@
         <v>49.6</v>
       </c>
       <c r="AP5">
-        <v>91.90000000000001</v>
+        <v>91.9</v>
       </c>
       <c r="AQ5">
         <v>98.3</v>
@@ -1522,7 +1535,7 @@
         <v>92.5</v>
       </c>
       <c r="AW5">
-        <v>97.09999999999999</v>
+        <v>97.1</v>
       </c>
       <c r="AX5">
         <v>101</v>
@@ -1546,28 +1559,28 @@
         <v>109.2</v>
       </c>
       <c r="BF5">
-        <v>2.5485</v>
+        <v>2.5485000000000002</v>
       </c>
       <c r="BG5">
-        <v>2.333791208791209</v>
+        <v>2.3337912087912089</v>
       </c>
       <c r="BH5">
-        <v>0.8614000000000001</v>
+        <v>0.86140000000000005</v>
       </c>
       <c r="BI5">
-        <v>0.7888278388278389</v>
+        <v>0.78882783882783891</v>
       </c>
       <c r="BJ5">
-        <v>2.958555839331321</v>
+        <v>2.9585558393313209</v>
       </c>
       <c r="BL5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BM5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:66">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1074</v>
       </c>
@@ -1581,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6">
         <v>38.5</v>
@@ -1611,7 +1624,7 @@
         <v>2.81</v>
       </c>
       <c r="O6">
-        <v>4.831</v>
+        <v>4.8310000000000004</v>
       </c>
       <c r="P6">
         <v>3.99</v>
@@ -1644,7 +1657,7 @@
         <v>139.5</v>
       </c>
       <c r="Z6">
-        <v>171.3333333333333</v>
+        <v>171.33333333333329</v>
       </c>
       <c r="AA6">
         <v>51.5</v>
@@ -1659,22 +1672,22 @@
         <v>38.5</v>
       </c>
       <c r="AE6">
-        <v>7.387</v>
+        <v>7.3869999999999996</v>
       </c>
       <c r="AF6">
-        <v>2.765</v>
+        <v>2.7650000000000001</v>
       </c>
       <c r="AG6">
-        <v>1.392</v>
+        <v>1.3919999999999999</v>
       </c>
       <c r="AH6">
-        <v>2.571</v>
+        <v>2.5710000000000002</v>
       </c>
       <c r="AI6">
         <v>1.81</v>
       </c>
       <c r="AJ6">
-        <v>8.186999999999999</v>
+        <v>8.1869999999999994</v>
       </c>
       <c r="AK6">
         <v>14.11</v>
@@ -1710,7 +1723,7 @@
         <v>93.2</v>
       </c>
       <c r="AV6">
-        <v>95.59999999999999</v>
+        <v>95.6</v>
       </c>
       <c r="AW6">
         <v>100.5</v>
@@ -1737,31 +1750,28 @@
         <v>110.4</v>
       </c>
       <c r="BF6">
-        <v>2.506</v>
+        <v>2.5059999999999998</v>
       </c>
       <c r="BG6">
-        <v>2.269927536231884</v>
+        <v>2.2699275362318838</v>
       </c>
       <c r="BH6">
-        <v>0.7164</v>
+        <v>0.71640000000000004</v>
       </c>
       <c r="BI6">
-        <v>0.6489130434782608</v>
+        <v>0.64891304347826084</v>
       </c>
       <c r="BJ6">
-        <v>3.498045784477945</v>
+        <v>3.4980457844779451</v>
       </c>
       <c r="BK6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL6" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:66">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1075</v>
       </c>
@@ -1796,10 +1806,10 @@
         <v>59782.5</v>
       </c>
       <c r="M7">
-        <v>1.846</v>
+        <v>1.8460000000000001</v>
       </c>
       <c r="N7">
-        <v>1.388</v>
+        <v>1.3879999999999999</v>
       </c>
       <c r="O7">
         <v>1.617</v>
@@ -1808,7 +1818,7 @@
         <v>1.71</v>
       </c>
       <c r="Q7">
-        <v>0.9908</v>
+        <v>0.99080000000000001</v>
       </c>
       <c r="R7">
         <v>1.123</v>
@@ -1850,31 +1860,31 @@
         <v>169</v>
       </c>
       <c r="AE7">
-        <v>2.039</v>
+        <v>2.0390000000000001</v>
       </c>
       <c r="AF7">
         <v>1.476</v>
       </c>
       <c r="AG7">
-        <v>1.063</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="AH7">
         <v>1.603</v>
       </c>
       <c r="AI7">
-        <v>1.846</v>
+        <v>1.8460000000000001</v>
       </c>
       <c r="AJ7">
-        <v>2.708</v>
+        <v>2.7080000000000002</v>
       </c>
       <c r="AK7">
-        <v>2.297</v>
+        <v>2.2970000000000002</v>
       </c>
       <c r="AL7">
-        <v>3.373</v>
+        <v>3.3730000000000002</v>
       </c>
       <c r="AM7">
-        <v>3.086</v>
+        <v>3.0859999999999999</v>
       </c>
       <c r="AN7">
         <v>11.62</v>
@@ -1901,7 +1911,7 @@
         <v>86.7</v>
       </c>
       <c r="AV7">
-        <v>89.40000000000001</v>
+        <v>89.4</v>
       </c>
       <c r="AW7">
         <v>93</v>
@@ -1913,7 +1923,7 @@
         <v>105.5</v>
       </c>
       <c r="AZ7">
-        <v>90.90000000000001</v>
+        <v>90.9</v>
       </c>
       <c r="BA7">
         <v>93.2</v>
@@ -1931,25 +1941,25 @@
         <v>1.3107</v>
       </c>
       <c r="BG7">
-        <v>1.242369668246445</v>
+        <v>1.2423696682464449</v>
       </c>
       <c r="BH7">
-        <v>0.591</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="BI7">
-        <v>0.5601895734597157</v>
+        <v>0.56018957345971565</v>
       </c>
       <c r="BJ7">
-        <v>2.217766497461929</v>
+        <v>2.2177664974619291</v>
       </c>
       <c r="BK7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BL7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:66">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1076</v>
       </c>
@@ -1963,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8">
         <v>138</v>
@@ -1990,19 +2000,19 @@
         <v>2.827</v>
       </c>
       <c r="N8">
-        <v>2.017</v>
+        <v>2.0169999999999999</v>
       </c>
       <c r="O8">
-        <v>1.297</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="P8">
-        <v>1.543</v>
+        <v>1.5429999999999999</v>
       </c>
       <c r="Q8">
-        <v>2.076</v>
+        <v>2.0760000000000001</v>
       </c>
       <c r="R8">
-        <v>2.215</v>
+        <v>2.2149999999999999</v>
       </c>
       <c r="S8">
         <v>238.005</v>
@@ -2011,7 +2021,7 @@
         <v>96</v>
       </c>
       <c r="U8">
-        <v>387.6666666666667</v>
+        <v>387.66666666666669</v>
       </c>
       <c r="V8">
         <v>281</v>
@@ -2026,7 +2036,7 @@
         <v>435.5</v>
       </c>
       <c r="Z8">
-        <v>174.3333333333333</v>
+        <v>174.33333333333329</v>
       </c>
       <c r="AA8">
         <v>78.5</v>
@@ -2041,7 +2051,7 @@
         <v>138</v>
       </c>
       <c r="AE8">
-        <v>5.183</v>
+        <v>5.1829999999999998</v>
       </c>
       <c r="AF8">
         <v>2.09</v>
@@ -2050,22 +2060,22 @@
         <v>1.2</v>
       </c>
       <c r="AH8">
-        <v>1.824</v>
+        <v>1.8240000000000001</v>
       </c>
       <c r="AI8">
         <v>2.827</v>
       </c>
       <c r="AJ8">
-        <v>2.845</v>
+        <v>2.8450000000000002</v>
       </c>
       <c r="AK8">
-        <v>3.697</v>
+        <v>3.6970000000000001</v>
       </c>
       <c r="AL8">
         <v>3.637</v>
       </c>
       <c r="AM8">
-        <v>2.937</v>
+        <v>2.9369999999999998</v>
       </c>
       <c r="AN8">
         <v>16.37</v>
@@ -2074,10 +2084,10 @@
         <v>60.7</v>
       </c>
       <c r="AP8">
-        <v>95.40000000000001</v>
+        <v>95.4</v>
       </c>
       <c r="AQ8">
-        <v>99.09999999999999</v>
+        <v>99.1</v>
       </c>
       <c r="AR8">
         <v>106.3</v>
@@ -2089,10 +2099,10 @@
         <v>110.7</v>
       </c>
       <c r="AU8">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="AV8">
-        <v>94.90000000000001</v>
+        <v>94.9</v>
       </c>
       <c r="AW8">
         <v>99.5</v>
@@ -2125,25 +2135,22 @@
         <v>1.27850133809099</v>
       </c>
       <c r="BH8">
-        <v>0.696</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="BI8">
-        <v>0.6208742194469223</v>
+        <v>0.62087421944692234</v>
       </c>
       <c r="BJ8">
         <v>2.059195402298851</v>
       </c>
       <c r="BK8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BL8" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:66">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1080</v>
       </c>
@@ -2157,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>4.951</v>
+        <v>4.9509999999999996</v>
       </c>
       <c r="T9">
         <v>57</v>
@@ -2190,7 +2197,7 @@
         <v>52</v>
       </c>
       <c r="AE9">
-        <v>2.132</v>
+        <v>2.1320000000000001</v>
       </c>
       <c r="AF9">
         <v>1.875</v>
@@ -2199,10 +2206,10 @@
         <v>1.29</v>
       </c>
       <c r="AH9">
-        <v>1.934</v>
+        <v>1.9339999999999999</v>
       </c>
       <c r="AI9">
-        <v>4.951</v>
+        <v>4.9509999999999996</v>
       </c>
       <c r="AJ9">
         <v>10.52</v>
@@ -2211,7 +2218,7 @@
         <v>12.96</v>
       </c>
       <c r="AL9">
-        <v>4.553</v>
+        <v>4.5529999999999999</v>
       </c>
       <c r="AM9">
         <v>16.79</v>
@@ -2220,7 +2227,7 @@
         <v>48.7</v>
       </c>
       <c r="AP9">
-        <v>94.90000000000001</v>
+        <v>94.9</v>
       </c>
       <c r="AQ9">
         <v>102</v>
@@ -2247,7 +2254,7 @@
         <v>112.1</v>
       </c>
       <c r="AZ9">
-        <v>91.40000000000001</v>
+        <v>91.4</v>
       </c>
       <c r="BA9">
         <v>101</v>
@@ -2262,28 +2269,28 @@
         <v>112.1</v>
       </c>
       <c r="BF9">
-        <v>1.9369</v>
+        <v>1.9369000000000001</v>
       </c>
       <c r="BG9">
-        <v>1.727832292595897</v>
+        <v>1.7278322925958971</v>
       </c>
       <c r="BH9">
-        <v>0.7754</v>
+        <v>0.77539999999999998</v>
       </c>
       <c r="BI9">
         <v>0.6917038358608385</v>
       </c>
       <c r="BJ9">
-        <v>2.497936548877999</v>
+        <v>2.4979365488779992</v>
       </c>
       <c r="BL9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BM9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:66">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1081</v>
       </c>
@@ -2318,7 +2325,7 @@
         <v>59965</v>
       </c>
       <c r="M10">
-        <v>2.043</v>
+        <v>2.0430000000000001</v>
       </c>
       <c r="N10">
         <v>1.54</v>
@@ -2330,10 +2337,10 @@
         <v>2.976</v>
       </c>
       <c r="Q10">
-        <v>1.249</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="R10">
-        <v>1.561</v>
+        <v>1.5609999999999999</v>
       </c>
       <c r="S10">
         <v>204.07</v>
@@ -2342,7 +2349,7 @@
         <v>79</v>
       </c>
       <c r="U10">
-        <v>297.3333333333333</v>
+        <v>297.33333333333331</v>
       </c>
       <c r="V10">
         <v>326.5</v>
@@ -2372,19 +2379,19 @@
         <v>171</v>
       </c>
       <c r="AE10">
-        <v>4.534</v>
+        <v>4.5339999999999998</v>
       </c>
       <c r="AF10">
-        <v>8.913</v>
+        <v>8.9130000000000003</v>
       </c>
       <c r="AG10">
-        <v>2.239</v>
+        <v>2.2389999999999999</v>
       </c>
       <c r="AH10">
-        <v>1.725</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="AI10">
-        <v>2.043</v>
+        <v>2.0430000000000001</v>
       </c>
       <c r="AJ10">
         <v>3.96</v>
@@ -2393,10 +2400,10 @@
         <v>6.798</v>
       </c>
       <c r="AL10">
-        <v>5.126</v>
+        <v>5.1260000000000003</v>
       </c>
       <c r="AM10">
-        <v>3.001</v>
+        <v>3.0009999999999999</v>
       </c>
       <c r="AN10">
         <v>14.42</v>
@@ -2420,13 +2427,13 @@
         <v>109.2</v>
       </c>
       <c r="AU10">
-        <v>90.59999999999999</v>
+        <v>90.6</v>
       </c>
       <c r="AV10">
-        <v>95.09999999999999</v>
+        <v>95.1</v>
       </c>
       <c r="AW10">
-        <v>99.59999999999999</v>
+        <v>99.6</v>
       </c>
       <c r="AX10">
         <v>102.9</v>
@@ -2456,22 +2463,22 @@
         <v>1.193551236749117</v>
       </c>
       <c r="BH10">
-        <v>0.6283</v>
+        <v>0.62829999999999997</v>
       </c>
       <c r="BI10">
-        <v>0.5550353356890459</v>
+        <v>0.55503533568904595</v>
       </c>
       <c r="BJ10">
         <v>2.150405857074646</v>
       </c>
       <c r="BK10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BL10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:66">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1082</v>
       </c>
@@ -2485,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11">
         <v>62</v>
@@ -2509,22 +2516,22 @@
         <v>56462.5</v>
       </c>
       <c r="M11">
-        <v>1.279</v>
+        <v>1.2789999999999999</v>
       </c>
       <c r="N11">
-        <v>1.443</v>
+        <v>1.4430000000000001</v>
       </c>
       <c r="O11">
-        <v>2.022</v>
+        <v>2.0219999999999998</v>
       </c>
       <c r="P11">
-        <v>1.398</v>
+        <v>1.3979999999999999</v>
       </c>
       <c r="Q11">
         <v>1.347</v>
       </c>
       <c r="R11">
-        <v>2.301</v>
+        <v>2.3010000000000002</v>
       </c>
       <c r="S11">
         <v>198.65</v>
@@ -2551,7 +2558,7 @@
         <v>59</v>
       </c>
       <c r="AA11">
-        <v>53.33333333333334</v>
+        <v>53.333333333333343</v>
       </c>
       <c r="AB11">
         <v>50</v>
@@ -2563,7 +2570,7 @@
         <v>62</v>
       </c>
       <c r="AE11">
-        <v>2.324</v>
+        <v>2.3239999999999998</v>
       </c>
       <c r="AG11">
         <v>1.119</v>
@@ -2572,16 +2579,16 @@
         <v>1.389</v>
       </c>
       <c r="AI11">
-        <v>1.279</v>
+        <v>1.2789999999999999</v>
       </c>
       <c r="AJ11">
-        <v>4.588</v>
+        <v>4.5880000000000001</v>
       </c>
       <c r="AK11">
-        <v>2.971</v>
+        <v>2.9710000000000001</v>
       </c>
       <c r="AL11">
-        <v>3.465</v>
+        <v>3.4649999999999999</v>
       </c>
       <c r="AM11">
         <v>2.145</v>
@@ -2593,7 +2600,7 @@
         <v>54.1</v>
       </c>
       <c r="AP11">
-        <v>95.90000000000001</v>
+        <v>95.9</v>
       </c>
       <c r="AQ11">
         <v>102</v>
@@ -2608,16 +2615,16 @@
         <v>105.5</v>
       </c>
       <c r="AU11">
-        <v>89.59999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="AV11">
         <v>93.8</v>
       </c>
       <c r="AW11">
-        <v>98.40000000000001</v>
+        <v>98.4</v>
       </c>
       <c r="AX11">
-        <v>99.90000000000001</v>
+        <v>99.9</v>
       </c>
       <c r="AY11">
         <v>108.8</v>
@@ -2638,31 +2645,28 @@
         <v>108.8</v>
       </c>
       <c r="BF11">
-        <v>0.8904</v>
+        <v>0.89039999999999997</v>
       </c>
       <c r="BG11">
-        <v>0.8183823529411764</v>
+        <v>0.81838235294117645</v>
       </c>
       <c r="BH11">
-        <v>0.6515</v>
+        <v>0.65149999999999997</v>
       </c>
       <c r="BI11">
-        <v>0.5988051470588235</v>
+        <v>0.59880514705882348</v>
       </c>
       <c r="BJ11">
-        <v>1.366692248656945</v>
+        <v>1.3666922486569451</v>
       </c>
       <c r="BK11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BL11" t="s">
-        <v>74</v>
-      </c>
-      <c r="BN11" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:66">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1091</v>
       </c>
@@ -2676,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <v>72</v>
@@ -2706,16 +2710,16 @@
         <v>5.008</v>
       </c>
       <c r="O12">
-        <v>6.969</v>
+        <v>6.9690000000000003</v>
       </c>
       <c r="P12">
-        <v>5.861</v>
+        <v>5.8609999999999998</v>
       </c>
       <c r="Q12">
-        <v>8.509</v>
+        <v>8.5090000000000003</v>
       </c>
       <c r="R12">
-        <v>0.905</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="S12">
         <v>653.495</v>
@@ -2739,7 +2743,7 @@
         <v>68</v>
       </c>
       <c r="Z12">
-        <v>53.33333333333334</v>
+        <v>53.333333333333343</v>
       </c>
       <c r="AA12">
         <v>63</v>
@@ -2754,7 +2758,7 @@
         <v>72</v>
       </c>
       <c r="AE12">
-        <v>0.9529</v>
+        <v>0.95289999999999997</v>
       </c>
       <c r="AF12">
         <v>1.758</v>
@@ -2781,7 +2785,7 @@
         <v>17.55</v>
       </c>
       <c r="AN12">
-        <v>8.289999999999999</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="AO12">
         <v>41.1</v>
@@ -2790,7 +2794,7 @@
         <v>78.5</v>
       </c>
       <c r="AQ12">
-        <v>83.09999999999999</v>
+        <v>83.1</v>
       </c>
       <c r="AR12">
         <v>87.3</v>
@@ -2799,10 +2803,10 @@
         <v>89.5</v>
       </c>
       <c r="AT12">
-        <v>89.59999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="AU12">
-        <v>70.90000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="AV12">
         <v>75.8</v>
@@ -2814,10 +2818,10 @@
         <v>83.8</v>
       </c>
       <c r="AY12">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="AZ12">
-        <v>76.09999999999999</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="BA12">
         <v>81.2</v>
@@ -2829,34 +2833,31 @@
         <v>89</v>
       </c>
       <c r="BD12">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="BF12">
-        <v>1.493</v>
+        <v>1.4930000000000001</v>
       </c>
       <c r="BG12">
         <v>1.615800865800866</v>
       </c>
       <c r="BH12">
-        <v>0.5354</v>
+        <v>0.53539999999999999</v>
       </c>
       <c r="BI12">
-        <v>0.5794372294372294</v>
+        <v>0.57943722943722942</v>
       </c>
       <c r="BJ12">
-        <v>2.788569293985805</v>
+        <v>2.7885692939858049</v>
       </c>
       <c r="BK12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL12" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN12" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:66">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1092</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13">
         <v>59.5</v>
@@ -2897,19 +2898,19 @@
         <v>3.29</v>
       </c>
       <c r="N13">
-        <v>5.481</v>
+        <v>5.4809999999999999</v>
       </c>
       <c r="O13">
-        <v>6.564</v>
+        <v>6.5640000000000001</v>
       </c>
       <c r="P13">
-        <v>6.934</v>
+        <v>6.9340000000000002</v>
       </c>
       <c r="Q13">
         <v>17.88</v>
       </c>
       <c r="R13">
-        <v>7.879</v>
+        <v>7.8789999999999996</v>
       </c>
       <c r="S13">
         <v>1316.55</v>
@@ -2948,28 +2949,28 @@
         <v>59.5</v>
       </c>
       <c r="AE13">
-        <v>0.4745</v>
+        <v>0.47449999999999998</v>
       </c>
       <c r="AF13">
         <v>1.18</v>
       </c>
       <c r="AG13">
-        <v>1.055</v>
+        <v>1.0549999999999999</v>
       </c>
       <c r="AH13">
-        <v>2.123</v>
+        <v>2.1230000000000002</v>
       </c>
       <c r="AI13">
         <v>3.29</v>
       </c>
       <c r="AJ13">
-        <v>8.537000000000001</v>
+        <v>8.5370000000000008</v>
       </c>
       <c r="AK13">
-        <v>16.69</v>
+        <v>16.690000000000001</v>
       </c>
       <c r="AL13">
-        <v>19.33</v>
+        <v>19.329999999999998</v>
       </c>
       <c r="AM13">
         <v>15.15</v>
@@ -2987,7 +2988,7 @@
         <v>84.2</v>
       </c>
       <c r="AR13">
-        <v>87.59999999999999</v>
+        <v>87.6</v>
       </c>
       <c r="AS13">
         <v>91</v>
@@ -2999,7 +3000,7 @@
         <v>69.7</v>
       </c>
       <c r="AV13">
-        <v>75.09999999999999</v>
+        <v>75.099999999999994</v>
       </c>
       <c r="AW13">
         <v>84.2</v>
@@ -3032,25 +3033,22 @@
         <v>1.312512716174975</v>
       </c>
       <c r="BH13">
-        <v>0.6312</v>
+        <v>0.63119999999999998</v>
       </c>
       <c r="BI13">
-        <v>0.642115971515768</v>
+        <v>0.64211597151576805</v>
       </c>
       <c r="BJ13">
         <v>2.04404309252218</v>
       </c>
       <c r="BK13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL13" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:66">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1093</v>
       </c>
@@ -3064,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14">
         <v>50</v>
@@ -3091,22 +3089,22 @@
         <v>1.107</v>
       </c>
       <c r="N14">
-        <v>4.831</v>
+        <v>4.8310000000000004</v>
       </c>
       <c r="O14">
-        <v>2.626</v>
+        <v>2.6259999999999999</v>
       </c>
       <c r="P14">
         <v>2.31</v>
       </c>
       <c r="Q14">
-        <v>5.872</v>
+        <v>5.8719999999999999</v>
       </c>
       <c r="R14">
-        <v>2.098</v>
+        <v>2.0979999999999999</v>
       </c>
       <c r="S14">
-        <v>453.485</v>
+        <v>453.48500000000001</v>
       </c>
       <c r="T14">
         <v>72</v>
@@ -3142,16 +3140,16 @@
         <v>50</v>
       </c>
       <c r="AE14">
-        <v>0.8927</v>
+        <v>0.89270000000000005</v>
       </c>
       <c r="AF14">
-        <v>0.9694</v>
+        <v>0.96940000000000004</v>
       </c>
       <c r="AG14">
-        <v>1.257</v>
+        <v>1.2569999999999999</v>
       </c>
       <c r="AH14">
-        <v>1.249</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="AI14">
         <v>1.107</v>
@@ -3166,10 +3164,10 @@
         <v>12.91</v>
       </c>
       <c r="AM14">
-        <v>9.305999999999999</v>
+        <v>9.3059999999999992</v>
       </c>
       <c r="AN14">
-        <v>9.640000000000001</v>
+        <v>9.64</v>
       </c>
       <c r="AO14">
         <v>41.3</v>
@@ -3178,7 +3176,7 @@
         <v>78.5</v>
       </c>
       <c r="AQ14">
-        <v>82.90000000000001</v>
+        <v>82.9</v>
       </c>
       <c r="AR14">
         <v>87.2</v>
@@ -3190,22 +3188,22 @@
         <v>92.3</v>
       </c>
       <c r="AU14">
-        <v>71.40000000000001</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="AV14">
-        <v>75.59999999999999</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="AW14">
-        <v>82.09999999999999</v>
+        <v>82.1</v>
       </c>
       <c r="AX14">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="AY14">
         <v>94.5</v>
       </c>
       <c r="AZ14">
-        <v>75.59999999999999</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="BA14">
         <v>81</v>
@@ -3214,7 +3212,7 @@
         <v>85.7</v>
       </c>
       <c r="BC14">
-        <v>90.40000000000001</v>
+        <v>90.4</v>
       </c>
       <c r="BD14">
         <v>94.5</v>
@@ -3226,25 +3224,22 @@
         <v>1.203597883597884</v>
       </c>
       <c r="BH14">
-        <v>0.5462</v>
+        <v>0.54620000000000002</v>
       </c>
       <c r="BI14">
-        <v>0.5779894179894181</v>
+        <v>0.57798941798941805</v>
       </c>
       <c r="BJ14">
-        <v>2.082387403881362</v>
+        <v>2.0823874038813619</v>
       </c>
       <c r="BK14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL14" t="s">
-        <v>74</v>
-      </c>
-      <c r="BN14" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:66">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1094</v>
       </c>
@@ -3294,7 +3289,7 @@
         <v>67.5</v>
       </c>
       <c r="X15">
-        <v>98.33333333333333</v>
+        <v>98.333333333333329</v>
       </c>
       <c r="Y15">
         <v>70</v>
@@ -3315,7 +3310,7 @@
         <v>48</v>
       </c>
       <c r="AE15">
-        <v>3.134</v>
+        <v>3.1339999999999999</v>
       </c>
       <c r="AF15">
         <v>1.165</v>
@@ -3324,13 +3319,13 @@
         <v>0.97</v>
       </c>
       <c r="AH15">
-        <v>1.055</v>
+        <v>1.0549999999999999</v>
       </c>
       <c r="AI15">
         <v>1.177</v>
       </c>
       <c r="AJ15">
-        <v>33.55</v>
+        <v>33.549999999999997</v>
       </c>
       <c r="AK15">
         <v>17.12</v>
@@ -3345,22 +3340,22 @@
         <v>21.59</v>
       </c>
       <c r="AO15">
-        <v>40.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="AP15">
         <v>80</v>
       </c>
       <c r="AQ15">
-        <v>85.09999999999999</v>
+        <v>85.1</v>
       </c>
       <c r="AR15">
         <v>89.5</v>
       </c>
       <c r="AS15">
-        <v>93.90000000000001</v>
+        <v>93.9</v>
       </c>
       <c r="AT15">
-        <v>94.40000000000001</v>
+        <v>94.4</v>
       </c>
       <c r="AU15">
         <v>73.5</v>
@@ -3372,7 +3367,7 @@
         <v>82.3</v>
       </c>
       <c r="AX15">
-        <v>87.40000000000001</v>
+        <v>87.4</v>
       </c>
       <c r="AY15">
         <v>98</v>
@@ -3381,40 +3376,40 @@
         <v>76.7</v>
       </c>
       <c r="BA15">
-        <v>82.90000000000001</v>
+        <v>82.9</v>
       </c>
       <c r="BB15">
-        <v>88.40000000000001</v>
+        <v>88.4</v>
       </c>
       <c r="BC15">
-        <v>93.40000000000001</v>
+        <v>93.4</v>
       </c>
       <c r="BD15">
         <v>98</v>
       </c>
       <c r="BF15">
-        <v>1.5393</v>
+        <v>1.5392999999999999</v>
       </c>
       <c r="BG15">
         <v>1.570714285714286</v>
       </c>
       <c r="BH15">
-        <v>0.641</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="BI15">
-        <v>0.6540816326530612</v>
+        <v>0.65408163265306118</v>
       </c>
       <c r="BJ15">
-        <v>2.401404056162247</v>
+        <v>2.4014040561622472</v>
       </c>
       <c r="BK15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:66">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1095</v>
       </c>
@@ -3449,25 +3444,25 @@
         <v>42057.5</v>
       </c>
       <c r="M16">
-        <v>4.525</v>
+        <v>4.5250000000000004</v>
       </c>
       <c r="N16">
-        <v>4.078</v>
+        <v>4.0780000000000003</v>
       </c>
       <c r="O16">
-        <v>8.012</v>
+        <v>8.0120000000000005</v>
       </c>
       <c r="P16">
-        <v>7.018</v>
+        <v>7.0179999999999998</v>
       </c>
       <c r="Q16">
-        <v>10.05</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="R16">
-        <v>6.535</v>
+        <v>6.5350000000000001</v>
       </c>
       <c r="S16">
-        <v>932.1849999999999</v>
+        <v>932.18499999999995</v>
       </c>
       <c r="T16">
         <v>81</v>
@@ -3476,7 +3471,7 @@
         <v>84</v>
       </c>
       <c r="V16">
-        <v>73.33333333333333</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="W16">
         <v>77</v>
@@ -3503,19 +3498,19 @@
         <v>43</v>
       </c>
       <c r="AE16">
-        <v>1.933</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="AF16">
-        <v>2.502</v>
+        <v>2.5019999999999998</v>
       </c>
       <c r="AG16">
-        <v>2.493</v>
+        <v>2.4929999999999999</v>
       </c>
       <c r="AH16">
-        <v>3.167</v>
+        <v>3.1669999999999998</v>
       </c>
       <c r="AI16">
-        <v>4.525</v>
+        <v>4.5250000000000004</v>
       </c>
       <c r="AJ16">
         <v>23.9</v>
@@ -3539,10 +3534,10 @@
         <v>82.5</v>
       </c>
       <c r="AQ16">
-        <v>87.59999999999999</v>
+        <v>87.6</v>
       </c>
       <c r="AR16">
-        <v>90.90000000000001</v>
+        <v>90.9</v>
       </c>
       <c r="AS16">
         <v>94.8</v>
@@ -3551,13 +3546,13 @@
         <v>94.8</v>
       </c>
       <c r="AU16">
-        <v>76.59999999999999</v>
+        <v>76.599999999999994</v>
       </c>
       <c r="AV16">
-        <v>81.59999999999999</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="AW16">
-        <v>85.90000000000001</v>
+        <v>85.9</v>
       </c>
       <c r="AX16">
         <v>89.2</v>
@@ -3566,10 +3561,10 @@
         <v>98.3</v>
       </c>
       <c r="AZ16">
-        <v>79.40000000000001</v>
+        <v>79.400000000000006</v>
       </c>
       <c r="BA16">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="BB16">
         <v>91.7</v>
@@ -3581,31 +3576,31 @@
         <v>98.3</v>
       </c>
       <c r="BF16">
-        <v>1.747</v>
+        <v>1.7470000000000001</v>
       </c>
       <c r="BG16">
-        <v>1.777212614445575</v>
+        <v>1.7772126144455751</v>
       </c>
       <c r="BH16">
-        <v>0.6412</v>
+        <v>0.64119999999999999</v>
       </c>
       <c r="BI16">
-        <v>0.6522889114954222</v>
+        <v>0.65228891149542223</v>
       </c>
       <c r="BJ16">
-        <v>2.724578914535246</v>
+        <v>2.7245789145352459</v>
       </c>
       <c r="BK16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BM16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:66">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1096</v>
       </c>
@@ -3640,25 +3635,25 @@
         <v>41505</v>
       </c>
       <c r="M17">
-        <v>4.015</v>
+        <v>4.0149999999999997</v>
       </c>
       <c r="N17">
-        <v>5.292</v>
+        <v>5.2919999999999998</v>
       </c>
       <c r="O17">
-        <v>5.079</v>
+        <v>5.0789999999999997</v>
       </c>
       <c r="P17">
-        <v>4.417</v>
+        <v>4.4169999999999998</v>
       </c>
       <c r="Q17">
-        <v>5.233</v>
+        <v>5.2329999999999997</v>
       </c>
       <c r="R17">
-        <v>6.299</v>
+        <v>6.2990000000000004</v>
       </c>
       <c r="S17">
-        <v>636.579999999999</v>
+        <v>636.57999999999902</v>
       </c>
       <c r="T17">
         <v>70</v>
@@ -3685,28 +3680,28 @@
         <v>55</v>
       </c>
       <c r="AB17">
-        <v>76.33333333333333</v>
+        <v>76.333333333333329</v>
       </c>
       <c r="AC17">
-        <v>63.33333333333334</v>
+        <v>63.333333333333343</v>
       </c>
       <c r="AD17">
         <v>58.5</v>
       </c>
       <c r="AE17">
-        <v>2.518</v>
+        <v>2.5179999999999998</v>
       </c>
       <c r="AF17">
         <v>3.536</v>
       </c>
       <c r="AG17">
-        <v>3.642</v>
+        <v>3.6419999999999999</v>
       </c>
       <c r="AH17">
-        <v>2.329</v>
+        <v>2.3290000000000002</v>
       </c>
       <c r="AI17">
-        <v>4.015</v>
+        <v>4.0149999999999997</v>
       </c>
       <c r="AJ17">
         <v>17.88</v>
@@ -3730,10 +3725,10 @@
         <v>93.2</v>
       </c>
       <c r="AQ17">
-        <v>95.40000000000001</v>
+        <v>95.4</v>
       </c>
       <c r="AR17">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="AS17">
         <v>99.3</v>
@@ -3748,7 +3743,7 @@
         <v>88.5</v>
       </c>
       <c r="AW17">
-        <v>93.59999999999999</v>
+        <v>93.6</v>
       </c>
       <c r="AX17">
         <v>90.5</v>
@@ -3766,7 +3761,7 @@
         <v>98.5</v>
       </c>
       <c r="BC17">
-        <v>97.40000000000001</v>
+        <v>97.4</v>
       </c>
       <c r="BD17">
         <v>104.4</v>
@@ -3778,22 +3773,22 @@
         <v>1.119827586206896</v>
       </c>
       <c r="BH17">
-        <v>0.6014</v>
+        <v>0.60140000000000005</v>
       </c>
       <c r="BI17">
-        <v>0.5760536398467433</v>
+        <v>0.57605363984674329</v>
       </c>
       <c r="BJ17">
-        <v>1.943964083804456</v>
+        <v>1.9439640838044561</v>
       </c>
       <c r="BK17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BL17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:66">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1100</v>
       </c>
@@ -3816,7 +3811,7 @@
         <v>78.5</v>
       </c>
       <c r="Z18">
-        <v>61.33333333333334</v>
+        <v>61.333333333333343</v>
       </c>
       <c r="AA18">
         <v>58</v>
@@ -3825,16 +3820,16 @@
         <v>41.2</v>
       </c>
       <c r="AP18">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="AQ18">
-        <v>95.90000000000001</v>
+        <v>95.9</v>
       </c>
       <c r="AU18">
         <v>85</v>
       </c>
       <c r="AV18">
-        <v>89.40000000000001</v>
+        <v>89.4</v>
       </c>
       <c r="AZ18">
         <v>89.7</v>
@@ -3843,10 +3838,10 @@
         <v>94.2</v>
       </c>
       <c r="BM18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:66">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1101</v>
       </c>
@@ -3860,7 +3855,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19">
         <v>64.5</v>
@@ -3884,25 +3879,25 @@
         <v>55007.5</v>
       </c>
       <c r="M19">
-        <v>0.9818</v>
+        <v>0.98180000000000001</v>
       </c>
       <c r="N19">
-        <v>0.8751</v>
+        <v>0.87509999999999999</v>
       </c>
       <c r="O19">
         <v>1.496</v>
       </c>
       <c r="P19">
-        <v>0.7983</v>
+        <v>0.79830000000000001</v>
       </c>
       <c r="Q19">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="R19">
         <v>1.919</v>
       </c>
       <c r="S19">
-        <v>153.906</v>
+        <v>153.90600000000001</v>
       </c>
       <c r="T19">
         <v>73</v>
@@ -3911,7 +3906,7 @@
         <v>459.5</v>
       </c>
       <c r="V19">
-        <v>342.6666666666667</v>
+        <v>342.66666666666669</v>
       </c>
       <c r="W19">
         <v>352</v>
@@ -3935,31 +3930,31 @@
         <v>64.5</v>
       </c>
       <c r="AE19">
-        <v>2.288</v>
+        <v>2.2879999999999998</v>
       </c>
       <c r="AF19">
-        <v>1.584</v>
+        <v>1.5840000000000001</v>
       </c>
       <c r="AG19">
         <v>1.982</v>
       </c>
       <c r="AH19">
-        <v>1.275</v>
+        <v>1.2749999999999999</v>
       </c>
       <c r="AI19">
-        <v>0.9818</v>
+        <v>0.98180000000000001</v>
       </c>
       <c r="AJ19">
-        <v>3.122</v>
+        <v>3.1219999999999999</v>
       </c>
       <c r="AK19">
         <v>4.12</v>
       </c>
       <c r="AL19">
-        <v>3.513</v>
+        <v>3.5129999999999999</v>
       </c>
       <c r="AM19">
-        <v>0.5975</v>
+        <v>0.59750000000000003</v>
       </c>
       <c r="AN19">
         <v>13.49</v>
@@ -3983,7 +3978,7 @@
         <v>88.2</v>
       </c>
       <c r="AV19">
-        <v>92.40000000000001</v>
+        <v>92.4</v>
       </c>
       <c r="AW19">
         <v>100.7</v>
@@ -3995,7 +3990,7 @@
         <v>110.5</v>
       </c>
       <c r="AZ19">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="BA19">
         <v>98.7</v>
@@ -4010,13 +4005,13 @@
         <v>110.5</v>
       </c>
       <c r="BF19">
-        <v>0.9262</v>
+        <v>0.92620000000000002</v>
       </c>
       <c r="BG19">
-        <v>0.8381900452488689</v>
+        <v>0.83819004524886886</v>
       </c>
       <c r="BH19">
-        <v>0.6216</v>
+        <v>0.62160000000000004</v>
       </c>
       <c r="BI19">
         <v>0.5625339366515838</v>
@@ -4025,16 +4020,13 @@
         <v>1.49002574002574</v>
       </c>
       <c r="BK19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL19" t="s">
-        <v>76</v>
-      </c>
-      <c r="BN19" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:66">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1102</v>
       </c>
@@ -4048,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F20">
         <v>48.5</v>
@@ -4072,7 +4064,7 @@
         <v>46565</v>
       </c>
       <c r="M20">
-        <v>2.777</v>
+        <v>2.7770000000000001</v>
       </c>
       <c r="N20">
         <v>3.512</v>
@@ -4081,13 +4073,13 @@
         <v>3.952</v>
       </c>
       <c r="P20">
-        <v>3.005</v>
+        <v>3.0049999999999999</v>
       </c>
       <c r="Q20">
         <v>2.919</v>
       </c>
       <c r="R20">
-        <v>3.235</v>
+        <v>3.2349999999999999</v>
       </c>
       <c r="S20">
         <v>377.03</v>
@@ -4108,13 +4100,13 @@
         <v>338.5</v>
       </c>
       <c r="Z20">
-        <v>39.33333333333334</v>
+        <v>39.333333333333343</v>
       </c>
       <c r="AA20">
         <v>41</v>
       </c>
       <c r="AB20">
-        <v>43.33333333333334</v>
+        <v>43.333333333333343</v>
       </c>
       <c r="AC20">
         <v>47</v>
@@ -4123,31 +4115,31 @@
         <v>48.5</v>
       </c>
       <c r="AE20">
-        <v>2.436</v>
+        <v>2.4359999999999999</v>
       </c>
       <c r="AF20">
         <v>2.633</v>
       </c>
       <c r="AG20">
-        <v>2.814</v>
+        <v>2.8140000000000001</v>
       </c>
       <c r="AH20">
-        <v>3.159</v>
+        <v>3.1589999999999998</v>
       </c>
       <c r="AI20">
-        <v>2.777</v>
+        <v>2.7770000000000001</v>
       </c>
       <c r="AJ20">
-        <v>8.574</v>
+        <v>8.5739999999999998</v>
       </c>
       <c r="AK20">
-        <v>5.433</v>
+        <v>5.4329999999999998</v>
       </c>
       <c r="AL20">
-        <v>9.151</v>
+        <v>9.1509999999999998</v>
       </c>
       <c r="AM20">
-        <v>6.909</v>
+        <v>6.9089999999999998</v>
       </c>
       <c r="AN20">
         <v>27.69</v>
@@ -4207,19 +4199,16 @@
         <v>0.878</v>
       </c>
       <c r="BI20">
-        <v>0.7238252267106348</v>
+        <v>0.72382522671063476</v>
       </c>
       <c r="BJ20">
         <v>1.942255125284738</v>
       </c>
       <c r="BK20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL20" t="s">
-        <v>75</v>
-      </c>
-      <c r="BN20" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>